<commit_message>
Add Pandas to virtual environment
</commit_message>
<xml_diff>
--- a/book_ans.xlsx
+++ b/book_ans.xlsx
@@ -16,7 +16,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="1">
+  <fonts count="2">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
@@ -24,13 +24,26 @@
       <sz val="12"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b val="1"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="0000ff00"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00ff3300"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -45,8 +58,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -424,7 +442,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H12"/>
+  <dimension ref="A1:H16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="D1" sqref="D1"/>
@@ -513,7 +531,7 @@
       <c r="C3" t="n">
         <v>80</v>
       </c>
-      <c r="D3" t="n">
+      <c r="D3" s="1" t="n">
         <v>40</v>
       </c>
       <c r="E3" t="n">
@@ -617,7 +635,7 @@
       <c r="C7" t="n">
         <v>40</v>
       </c>
-      <c r="D7" t="n">
+      <c r="D7" s="2" t="n">
         <v>20</v>
       </c>
       <c r="E7" t="n">
@@ -733,7 +751,7 @@
       <c r="G11" t="n">
         <v>2</v>
       </c>
-      <c r="H11" t="n">
+      <c r="H11" s="1" t="n">
         <v>40</v>
       </c>
     </row>
@@ -759,9 +777,25 @@
       <c r="G12" t="n">
         <v>1</v>
       </c>
-      <c r="H12" t="n">
+      <c r="H12" s="2" t="n">
         <v>20</v>
       </c>
+    </row>
+    <row r="15">
+      <c r="C15" s="3" t="inlineStr">
+        <is>
+          <t>Suitable</t>
+        </is>
+      </c>
+      <c r="D15" s="4" t="n"/>
+    </row>
+    <row r="16">
+      <c r="C16" s="3" t="inlineStr">
+        <is>
+          <t>Not Suitable</t>
+        </is>
+      </c>
+      <c r="D16" s="5" t="n"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>